<commit_message>
dialogdemo : simulation of answer store & disambiguation questions support
</commit_message>
<xml_diff>
--- a/fasttext/studies/Perf study.xlsx
+++ b/fasttext/studies/Perf study.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laurent\Downloads\fastText\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\ConversationTools\fasttext\studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="SAVINGS" sheetId="1" r:id="rId1"/>
+    <sheet name="INSURANCE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>bin</t>
   </si>
@@ -289,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +323,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +640,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +699,7 @@
         <v>-4.1666666666666288</v>
       </c>
       <c r="H2" s="2">
-        <f>AVERAGE(I2:O2)</f>
+        <f t="shared" ref="H2:H9" si="1">AVERAGE(I2:O2)</f>
         <v>785</v>
       </c>
       <c r="I2">
@@ -746,7 +748,7 @@
         <v>-2.3095238095237391</v>
       </c>
       <c r="H3" s="9">
-        <f>AVERAGE(I3:O3)</f>
+        <f t="shared" si="1"/>
         <v>786.85714285714289</v>
       </c>
       <c r="I3">
@@ -801,7 +803,7 @@
         <v>-9.1666666666666288</v>
       </c>
       <c r="H4" s="2">
-        <f>AVERAGE(I4:O4)</f>
+        <f t="shared" si="1"/>
         <v>780</v>
       </c>
       <c r="I4">
@@ -847,7 +849,7 @@
         <v>-7.5952380952380736</v>
       </c>
       <c r="H5" s="2">
-        <f>AVERAGE(I5:O5)</f>
+        <f t="shared" si="1"/>
         <v>781.57142857142856</v>
       </c>
       <c r="I5">
@@ -896,7 +898,7 @@
         <v>-7.0238095238095184</v>
       </c>
       <c r="H6" s="2">
-        <f>AVERAGE(I6:O6)</f>
+        <f t="shared" si="1"/>
         <v>782.14285714285711</v>
       </c>
       <c r="I6">
@@ -948,7 +950,7 @@
         <v>-7.1666666666666288</v>
       </c>
       <c r="H7" s="2">
-        <f>AVERAGE(I7:O7)</f>
+        <f t="shared" si="1"/>
         <v>782</v>
       </c>
       <c r="I7">
@@ -997,7 +999,7 @@
         <v>-185.73809523809518</v>
       </c>
       <c r="H8" s="2">
-        <f>AVERAGE(I8:O8)</f>
+        <f t="shared" si="1"/>
         <v>603.42857142857144</v>
       </c>
       <c r="I8">
@@ -1046,7 +1048,7 @@
         <v>-189.45238095238096</v>
       </c>
       <c r="H9" s="2">
-        <f>AVERAGE(I9:O9)</f>
+        <f t="shared" si="1"/>
         <v>599.71428571428567</v>
       </c>
       <c r="I9">
@@ -1091,7 +1093,7 @@
         <v>24</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" ref="G10:G21" si="1">H10-$H$10</f>
+        <f t="shared" ref="G10:G19" si="2">H10-$H$10</f>
         <v>0</v>
       </c>
       <c r="H10" s="4">
@@ -1143,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="H11" s="2">
@@ -1195,7 +1197,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.1666666666666288</v>
       </c>
       <c r="H12" s="2">
@@ -1241,11 +1243,11 @@
         <v>3</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.5</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" ref="H13:H17" si="2">AVERAGE(I13:N13)</f>
+        <f t="shared" ref="H13:H17" si="3">AVERAGE(I13:N13)</f>
         <v>781.66666666666663</v>
       </c>
       <c r="I13">
@@ -1290,11 +1292,11 @@
         <v>16</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-75.333333333333258</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>713.83333333333337</v>
       </c>
       <c r="I14">
@@ -1342,11 +1344,11 @@
         <v>2</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-73.333333333333258</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>715.83333333333337</v>
       </c>
       <c r="I15">
@@ -1391,11 +1393,11 @@
         <v>0.23</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-82.333333333333258</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>706.83333333333337</v>
       </c>
       <c r="I16">
@@ -1446,11 +1448,11 @@
         <v>0.23</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-82.333333333333258</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>706.83333333333337</v>
       </c>
       <c r="I17">
@@ -1504,7 +1506,7 @@
         <v>0.3</v>
       </c>
       <c r="G19" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-11.452380952380963</v>
       </c>
       <c r="H19" s="2">
@@ -1567,6 +1569,78 @@
       <c r="G23" s="16">
         <f>H19-$H$22</f>
         <v>-56.285714285714334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="20">
+        <f>AVERAGE(H2:N2)</f>
+        <v>684</v>
+      </c>
+      <c r="H2">
+        <v>682</v>
+      </c>
+      <c r="I2">
+        <v>695</v>
+      </c>
+      <c r="J2">
+        <v>679</v>
+      </c>
+      <c r="K2">
+        <v>697</v>
+      </c>
+      <c r="L2">
+        <v>678</v>
+      </c>
+      <c r="M2">
+        <v>709</v>
+      </c>
+      <c r="N2">
+        <v>648</v>
+      </c>
+      <c r="O2">
+        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>